<commit_message>
Order upgrade - second try at reformatting - add options for order
</commit_message>
<xml_diff>
--- a/data/input/trade/Book1.xlsx
+++ b/data/input/trade/Book1.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisareade/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biacarvalheira/Desktop/DEVELOPMENT/FREELANCER/excelWeb_script/data/input/trade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD331E36-D551-B14A-9188-A8CB3EA77D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AC7F7C-9BDE-8A41-9A99-A936631E82F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16660" xr2:uid="{DEE40ED8-3044-2E42-B923-264BF91B84B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>DATE</t>
   </si>
@@ -168,12 +168,6 @@
   </si>
   <si>
     <t>APO Mar 15 2024 85.0 Put</t>
-  </si>
-  <si>
-    <t>Bought 300 BNPQY @ 31.18</t>
-  </si>
-  <si>
-    <t>BNPQY</t>
   </si>
   <si>
     <t>Bought 2 TOST Feb 9 2024 16.5 Put @ 0.02</t>
@@ -306,9 +300,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -346,7 +340,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -452,7 +446,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -594,7 +588,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -602,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E586FF50-38EE-C349-8CA8-92BBE61D9CE5}">
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1135,24 +1129,24 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>45323</v>
+        <v>45324</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D21" s="3">
-        <v>300</v>
+        <v>2</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F21" s="3">
-        <v>31.18</v>
+        <v>0.02</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3">
-        <v>-9359</v>
+        <v>-4.0199999999999996</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="4"/>
@@ -1168,17 +1162,17 @@
         <v>46</v>
       </c>
       <c r="D22" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F22" s="3">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3">
-        <v>-4.0199999999999996</v>
+        <v>-5.01</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="4"/>
@@ -1194,17 +1188,17 @@
         <v>48</v>
       </c>
       <c r="D23" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F23" s="3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3">
-        <v>-5.01</v>
+        <v>-24.07</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="4"/>
@@ -1217,20 +1211,20 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="3">
         <v>6</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F24" s="3">
-        <v>0.04</v>
+        <v>0.19</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3">
-        <v>-24.07</v>
+        <v>110.61</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="4"/>
@@ -1246,17 +1240,17 @@
         <v>51</v>
       </c>
       <c r="D25" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F25" s="3">
-        <v>0.19</v>
+        <v>1.56</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3">
-        <v>110.61</v>
+        <v>155.44</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="4"/>
@@ -1278,11 +1272,11 @@
         <v>54</v>
       </c>
       <c r="F26" s="3">
-        <v>1.56</v>
+        <v>0.54</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3">
-        <v>155.44</v>
+        <v>-54.56</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="4"/>
@@ -1304,13 +1298,13 @@
         <v>56</v>
       </c>
       <c r="F27" s="3">
-        <v>0.54</v>
+        <v>0.77</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3">
-        <v>-54.56</v>
-      </c>
-      <c r="I27" s="3"/>
+        <v>76.44</v>
+      </c>
+      <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -1324,17 +1318,17 @@
         <v>57</v>
       </c>
       <c r="D28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>58</v>
       </c>
       <c r="F28" s="3">
-        <v>0.77</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3">
-        <v>76.44</v>
+        <v>54.87</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -1350,17 +1344,17 @@
         <v>59</v>
       </c>
       <c r="D29" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>60</v>
       </c>
       <c r="F29" s="3">
-        <v>0.28000000000000003</v>
+        <v>1.26</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3">
-        <v>54.87</v>
+        <v>125.44</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -1368,42 +1362,22 @@
       <c r="L29" s="4"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>45324</v>
+      <c r="A30" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="3">
-        <v>1</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="3">
-        <v>1.26</v>
-      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="3">
-        <v>125.44</v>
-      </c>
+      <c r="H30" s="3"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -1416,7 +1390,15 @@
       <c r="L32" s="4"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I33" s="4"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -1428,9 +1410,9 @@
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="4"/>
+      <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
+      <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -1440,11 +1422,11 @@
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="E35" s="4"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
+      <c r="G35" s="4"/>
       <c r="H35" s="3"/>
-      <c r="I35" s="4"/>
+      <c r="I35" s="3"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -1468,9 +1450,9 @@
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="4"/>
+      <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="4"/>
+      <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="4"/>
@@ -1498,7 +1480,7 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+      <c r="G39" s="4"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="4"/>
@@ -1510,7 +1492,7 @@
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="E40" s="4"/>
       <c r="F40" s="3"/>
       <c r="G40" s="4"/>
       <c r="H40" s="3"/>
@@ -1520,28 +1502,20 @@
       <c r="L40" s="4"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
       <c r="E41" s="4"/>
-      <c r="F41" s="3"/>
+      <c r="F41" s="4"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
+      <c r="I42" s="3"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
@@ -1589,13 +1563,13 @@
       <c r="L49" s="4"/>
     </row>
     <row r="50" spans="9:12" x14ac:dyDescent="0.2">
-      <c r="I50" s="3"/>
+      <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
     </row>
     <row r="51" spans="9:12" x14ac:dyDescent="0.2">
-      <c r="I51" s="4"/>
+      <c r="I51" s="3"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
@@ -1613,7 +1587,7 @@
       <c r="L53" s="4"/>
     </row>
     <row r="54" spans="9:12" x14ac:dyDescent="0.2">
-      <c r="I54" s="3"/>
+      <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -1666,12 +1640,6 @@
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
     </row>
-    <row r="63" spans="9:12" x14ac:dyDescent="0.2">
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>